<commit_message>
adding Detainees n, some formatting edits
</commit_message>
<xml_diff>
--- a/Data/CCJ_quantified_values.xlsx
+++ b/Data/CCJ_quantified_values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larapesceares/CCJ/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636F6BC8-35D6-434D-8406-E7531BFBACC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6390E8-26B7-E84F-95B0-1BDE75FDA159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{B2B1E421-E324-4B4D-ACA9-CCF9679130E2}"/>
+    <workbookView xWindow="-10640" yWindow="-27980" windowWidth="44440" windowHeight="23800" xr2:uid="{B2B1E421-E324-4B4D-ACA9-CCF9679130E2}"/>
   </bookViews>
   <sheets>
     <sheet name="CCJ_quantified values" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="93">
   <si>
     <t>Component name</t>
   </si>
@@ -69,9 +69,6 @@
     <t>short run</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>negative</t>
   </si>
   <si>
@@ -295,13 +292,31 @@
   </si>
   <si>
     <t>dollars</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>n Detainees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n Society </t>
+  </si>
+  <si>
+    <t>https://cook-dashboard.loyolaccj.org/jail/admissions?utm_source=chatgpt.com</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>people</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -445,8 +460,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -624,6 +646,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -788,7 +816,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -799,6 +827,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1175,7 +1205,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995123B1-1625-034D-9BEA-A8F37EC1EE44}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
@@ -1192,77 +1222,77 @@
     <col min="14" max="14" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="O1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="R1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1273,19 +1303,19 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1296,19 +1326,19 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1317,15 +1347,15 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="P4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1345,16 +1375,16 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
@@ -1368,43 +1398,41 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="L7" s="3">
         <v>2018</v>
       </c>
       <c r="M7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -1412,13 +1440,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
@@ -1426,26 +1454,23 @@
       <c r="G8">
         <v>60.37</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="H8" s="3"/>
       <c r="I8" s="3">
         <v>60.37</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="N8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O8" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -1453,13 +1478,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
@@ -1470,26 +1495,25 @@
       <c r="H9" s="3">
         <v>0.61</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
       <c r="K9" s="3">
         <v>0.71</v>
       </c>
+      <c r="M9" t="s">
+        <v>12</v>
+      </c>
       <c r="O9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -1497,13 +1521,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -1517,20 +1541,19 @@
       <c r="I10" s="3">
         <v>33</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
       <c r="L10">
         <v>2011</v>
       </c>
+      <c r="M10" t="s">
+        <v>12</v>
+      </c>
       <c r="O10" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" t="s">
         <v>40</v>
-      </c>
-      <c r="P10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -1538,13 +1561,13 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -1552,26 +1575,23 @@
       <c r="G11">
         <v>4.9400000000000004</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="H11" s="3"/>
       <c r="I11" s="3">
         <v>4.9400000000000004</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="M11" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="N11" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" t="s">
         <v>51</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>52</v>
-      </c>
-      <c r="P11" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -1585,31 +1605,23 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12">
         <v>-99.44</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="M12" t="s">
         <v>12</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M12" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -1617,13 +1629,13 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -1631,29 +1643,23 @@
       <c r="G13">
         <v>-11</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="H13" s="3"/>
       <c r="I13" s="3">
         <v>11</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
       <c r="L13">
         <v>2022</v>
       </c>
       <c r="M13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O13" t="s">
+        <v>56</v>
+      </c>
+      <c r="P13" t="s">
         <v>57</v>
-      </c>
-      <c r="P13" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -1661,19 +1667,19 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G14" s="2">
         <v>-249634</v>
@@ -1681,12 +1687,8 @@
       <c r="H14" s="4">
         <v>178920</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="4">
         <v>249634</v>
       </c>
@@ -1694,30 +1696,30 @@
         <v>2021</v>
       </c>
       <c r="M14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O14" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14" t="s">
         <v>57</v>
-      </c>
-      <c r="P14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15">
         <v>130</v>
@@ -1728,28 +1730,31 @@
       <c r="L15">
         <v>2017</v>
       </c>
+      <c r="M15" t="s">
+        <v>87</v>
+      </c>
       <c r="N15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
@@ -1766,25 +1771,28 @@
       <c r="L16">
         <v>2015</v>
       </c>
+      <c r="M16" t="s">
+        <v>87</v>
+      </c>
       <c r="O16" t="s">
+        <v>70</v>
+      </c>
+      <c r="P16" t="s">
         <v>71</v>
-      </c>
-      <c r="P16" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -1798,28 +1806,31 @@
       <c r="K17">
         <v>400</v>
       </c>
+      <c r="M17" t="s">
+        <v>87</v>
+      </c>
       <c r="N17" t="s">
+        <v>78</v>
+      </c>
+      <c r="O17" t="s">
         <v>79</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>80</v>
-      </c>
-      <c r="P17" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -1829,6 +1840,40 @@
       </c>
       <c r="H18" s="5">
         <v>448677628</v>
+      </c>
+      <c r="M18" t="s">
+        <v>87</v>
+      </c>
+      <c r="O18" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19">
+        <v>33945</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first calculation in progress, debugging
</commit_message>
<xml_diff>
--- a/Data/CCJ_quantified_values.xlsx
+++ b/Data/CCJ_quantified_values.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/td/PycharmProjects/CCJ/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larapesceares/CCJ/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4391C82C-48EA-3F41-8B0A-19B4F4C40039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27B1467-66E2-7243-A15F-0B921763CFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="820" windowWidth="27180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="121">
   <si>
     <t>row_var</t>
   </si>
@@ -43,9 +43,6 @@
     <t>dependencies</t>
   </si>
   <si>
-    <t>selected value</t>
-  </si>
-  <si>
     <t>Min</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>Max</t>
   </si>
   <si>
-    <t>source dollar year</t>
-  </si>
-  <si>
     <t>impact</t>
   </si>
   <si>
@@ -154,15 +148,6 @@
     <t>dollar for 10 years</t>
   </si>
   <si>
-    <t>−3,677</t>
-  </si>
-  <si>
-    <t>−1,710</t>
-  </si>
-  <si>
-    <t>−5,623</t>
-  </si>
-  <si>
     <t>negative</t>
   </si>
   <si>
@@ -392,6 +377,12 @@
   </si>
   <si>
     <t>estimate</t>
+  </si>
+  <si>
+    <t>selected_value</t>
+  </si>
+  <si>
+    <t>source_dollar_year</t>
   </si>
 </sst>
 </file>
@@ -399,7 +390,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -449,10 +440,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -809,63 +800,63 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
       <c r="G2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -875,139 +866,139 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
       <c r="G3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H3" s="4">
+        <v>112</v>
+      </c>
+      <c r="H3" s="3">
         <v>973000</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>100000</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>973000</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>294728</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <v>10000000</v>
       </c>
       <c r="Q3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="3">
+        <v>875000</v>
+      </c>
+      <c r="I4" s="3">
+        <v>500000</v>
+      </c>
+      <c r="J4" s="3">
+        <v>875000</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3">
+        <v>1200000</v>
+      </c>
+      <c r="O4" t="s">
+        <v>113</v>
+      </c>
+      <c r="P4" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>123</v>
-      </c>
-      <c r="H4" s="4">
-        <v>875000</v>
-      </c>
-      <c r="I4" s="4">
-        <v>500000</v>
-      </c>
-      <c r="J4" s="4">
-        <v>875000</v>
-      </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="O4" t="s">
-        <v>118</v>
-      </c>
-      <c r="P4" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>31</v>
-      </c>
       <c r="R4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="S4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1015,71 +1006,71 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="P6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>45</v>
+      <c r="H7" s="2">
+        <v>3677</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1710</v>
       </c>
       <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>46</v>
+      <c r="K7" s="2">
+        <v>3677</v>
+      </c>
+      <c r="L7" s="2">
+        <v>5623</v>
       </c>
       <c r="M7">
         <v>2018</v>
       </c>
       <c r="N7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="P7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="3">
+        <v>34</v>
+      </c>
+      <c r="H8">
         <v>60.37</v>
       </c>
       <c r="I8" s="2"/>
@@ -1089,87 +1080,87 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="N8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="O8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="P8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="Q8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="3">
+        <v>34</v>
+      </c>
+      <c r="H9">
         <v>0.61</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9">
         <v>0.61</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="3">
+      <c r="L9">
         <v>0.71</v>
       </c>
       <c r="N9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="P9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="Q9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="R9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="S9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="3">
+        <v>34</v>
+      </c>
+      <c r="H10">
         <v>11</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10">
         <v>11</v>
       </c>
       <c r="J10" s="2">
@@ -1181,35 +1172,35 @@
         <v>2011</v>
       </c>
       <c r="N10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="P10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="Q10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="3">
+        <v>34</v>
+      </c>
+      <c r="H11">
         <v>4.9400000000000004</v>
       </c>
       <c r="I11" s="2"/>
@@ -1219,72 +1210,72 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="N11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="O11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="P11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>77</v>
-      </c>
-      <c r="H12" s="3">
-        <v>-99.44</v>
+        <v>72</v>
+      </c>
+      <c r="H12">
+        <v>99.44</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="N12" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="3">
-        <v>-11</v>
+        <v>34</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2">
@@ -1296,81 +1287,81 @@
         <v>2022</v>
       </c>
       <c r="N13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="P13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="Q13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" s="3">
-        <v>-249634</v>
-      </c>
-      <c r="I14" s="3">
+        <v>80</v>
+      </c>
+      <c r="H14">
+        <v>249634</v>
+      </c>
+      <c r="I14">
         <v>178920</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="3">
+      <c r="L14">
         <v>249634</v>
       </c>
       <c r="M14">
         <v>2021</v>
       </c>
       <c r="N14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="P14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="Q14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" t="s">
         <v>22</v>
       </c>
-      <c r="E15" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="3">
+      <c r="H15">
         <v>130</v>
       </c>
       <c r="I15" s="2"/>
@@ -1383,156 +1374,156 @@
         <v>2017</v>
       </c>
       <c r="N15" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="O15" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="Q15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="3">
+        <v>34</v>
+      </c>
+      <c r="H16">
         <v>50</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16">
         <v>25</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="3">
+      <c r="L16">
         <v>100</v>
       </c>
       <c r="M16">
         <v>2015</v>
       </c>
       <c r="N16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="P16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="Q16" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="3">
+        <v>34</v>
+      </c>
+      <c r="H17">
         <v>300</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17">
         <v>200</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="3">
+      <c r="L17">
         <v>400</v>
       </c>
       <c r="N17" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="O17" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="P17" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="Q17" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="3">
+        <v>34</v>
+      </c>
+      <c r="H18">
         <v>448677628</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18">
         <v>448677628</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="N18" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="P18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="Q18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E19" t="s">
-        <v>113</v>
-      </c>
-      <c r="H19" s="3">
+        <v>108</v>
+      </c>
+      <c r="H19">
         <v>33945</v>
       </c>
       <c r="I19" s="2"/>
@@ -1542,16 +1533,19 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E20" t="s">
-        <v>113</v>
+        <v>108</v>
+      </c>
+      <c r="H20" s="5">
+        <v>5171000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
short term societal values updated
</commit_message>
<xml_diff>
--- a/Data/CCJ_quantified_values.xlsx
+++ b/Data/CCJ_quantified_values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/td/PycharmProjects/CCJ/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832A8C5E-E9B5-AE44-9ACD-0897E55C4B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F426A1-33A6-9D42-8BFA-17896B92B641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="126">
   <si>
     <t>row_var</t>
   </si>
@@ -124,12 +124,6 @@
     <t>Short term value to society</t>
   </si>
   <si>
-    <t>Measure of crime prevented as a result of the detention</t>
-  </si>
-  <si>
-    <t>dollar</t>
-  </si>
-  <si>
     <t>short run</t>
   </si>
   <si>
@@ -392,6 +386,18 @@
   </si>
   <si>
     <t>estimate</t>
+  </si>
+  <si>
+    <t>https://loyolaccj.org/blog/cook-bond</t>
+  </si>
+  <si>
+    <t>Monetary D- bonds measuring the nature of crime, potential danger to public and danger of flee</t>
+  </si>
+  <si>
+    <t>Central bond court report 2018</t>
+  </si>
+  <si>
+    <t>https://cookcountysheriffil.gov/wp-content/uploads/2018/02/Central-Bond-Court-Report.pdf</t>
   </si>
 </sst>
 </file>
@@ -759,7 +765,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -864,7 +870,7 @@
         <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -892,7 +898,7 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H3" s="3">
         <v>973000</v>
@@ -910,7 +916,7 @@
         <v>10000000</v>
       </c>
       <c r="Q3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -927,13 +933,13 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H4" s="3">
         <v>875000</v>
@@ -949,19 +955,19 @@
         <v>1200000</v>
       </c>
       <c r="O4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="P4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Q4" t="s">
         <v>31</v>
       </c>
       <c r="R4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -972,41 +978,56 @@
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="H5" s="3">
+        <v>75000</v>
+      </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="J5" s="3">
+        <v>133685</v>
+      </c>
+      <c r="K5" s="3">
+        <v>75000</v>
+      </c>
       <c r="L5" s="3"/>
+      <c r="P5" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>125</v>
+      </c>
+      <c r="S5" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1014,69 +1035,69 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="P6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
         <v>40</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="M7">
         <v>2018</v>
       </c>
       <c r="N7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
         <v>49</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>50</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>51</v>
       </c>
-      <c r="D8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
-      </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H8">
         <v>60.37</v>
@@ -1088,36 +1109,36 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="N8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O8" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q8" t="s">
         <v>54</v>
-      </c>
-      <c r="P8" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
         <v>50</v>
       </c>
-      <c r="C9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" t="s">
-        <v>52</v>
-      </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H9">
         <v>0.61</v>
@@ -1131,39 +1152,39 @@
         <v>0.71</v>
       </c>
       <c r="N9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9" t="s">
         <v>59</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="S9" t="s">
         <v>60</v>
-      </c>
-      <c r="R9" t="s">
-        <v>61</v>
-      </c>
-      <c r="S9" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
         <v>63</v>
       </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" t="s">
-        <v>65</v>
-      </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H10">
         <v>11</v>
@@ -1180,33 +1201,33 @@
         <v>2011</v>
       </c>
       <c r="N10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
         <v>68</v>
       </c>
-      <c r="B11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" t="s">
-        <v>70</v>
-      </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H11">
         <v>4.9400000000000004</v>
@@ -1218,39 +1239,39 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="N11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q11" t="s">
         <v>71</v>
-      </c>
-      <c r="P11" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H12">
         <v>-99.44</v>
@@ -1260,27 +1281,27 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="N12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H13">
         <v>-11</v>
@@ -1295,36 +1316,36 @@
         <v>2022</v>
       </c>
       <c r="N13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="s">
         <v>82</v>
       </c>
-      <c r="B14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
         <v>83</v>
-      </c>
-      <c r="D14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" t="s">
-        <v>85</v>
       </c>
       <c r="H14">
         <v>-249634</v>
@@ -1341,30 +1362,30 @@
         <v>2021</v>
       </c>
       <c r="N14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
         <v>86</v>
-      </c>
-      <c r="B15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" t="s">
-        <v>88</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
         <v>24</v>
@@ -1382,36 +1403,36 @@
         <v>2017</v>
       </c>
       <c r="N15" t="s">
+        <v>88</v>
+      </c>
+      <c r="O15" t="s">
+        <v>89</v>
+      </c>
+      <c r="P15" t="s">
         <v>90</v>
       </c>
-      <c r="O15" t="s">
+      <c r="Q15" t="s">
         <v>91</v>
-      </c>
-      <c r="P15" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" t="s">
         <v>94</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>95</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>96</v>
       </c>
-      <c r="D16" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" t="s">
-        <v>98</v>
-      </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H16">
         <v>50</v>
@@ -1428,33 +1449,33 @@
         <v>2015</v>
       </c>
       <c r="N16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Q16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" t="s">
         <v>95</v>
-      </c>
-      <c r="C17" t="s">
-        <v>102</v>
-      </c>
-      <c r="D17" t="s">
-        <v>97</v>
       </c>
       <c r="E17" t="s">
         <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H17">
         <v>300</v>
@@ -1468,36 +1489,36 @@
         <v>400</v>
       </c>
       <c r="N17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O17" t="s">
+        <v>101</v>
+      </c>
+      <c r="P17" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q17" t="s">
         <v>103</v>
-      </c>
-      <c r="P17" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H18">
         <v>448677628</v>
@@ -1509,27 +1530,27 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="N18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" t="s">
         <v>110</v>
       </c>
-      <c r="B19" t="s">
+      <c r="E19" t="s">
         <v>111</v>
-      </c>
-      <c r="C19" t="s">
-        <v>112</v>
-      </c>
-      <c r="E19" t="s">
-        <v>113</v>
       </c>
       <c r="H19">
         <v>33945</v>
@@ -1541,16 +1562,16 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" t="s">
         <v>111</v>
-      </c>
-      <c r="C20" t="s">
-        <v>115</v>
-      </c>
-      <c r="E20" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculator, dash and values updated
</commit_message>
<xml_diff>
--- a/Data/CCJ_quantified_values.xlsx
+++ b/Data/CCJ_quantified_values.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larapesceares/CCJ/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/td/PycharmProjects/CCJ/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05952496-FD2F-594D-A937-9C865BD602C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1080FC-A4AB-AF4F-8266-2CF9ACE7E23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="133">
   <si>
     <t>row_var</t>
   </si>
@@ -94,15 +107,9 @@
     <t>Wrongful death damages Social cost of detainment and wtp for a human life</t>
   </si>
   <si>
-    <t>dollar per person</t>
-  </si>
-  <si>
     <t>haven_cost_of_crime</t>
   </si>
   <si>
-    <t>dollars per person</t>
-  </si>
-  <si>
     <t>https://nij.ojp.gov/library/publications/cost-crime-haven-conceptual-framework-measuring-victim-harms-violence</t>
   </si>
   <si>
@@ -404,6 +411,27 @@
   </si>
   <si>
     <t>dollars per day per person</t>
+  </si>
+  <si>
+    <t>multiple by length of stay</t>
+  </si>
+  <si>
+    <t>convert to day</t>
+  </si>
+  <si>
+    <t>dollar per detainee</t>
+  </si>
+  <si>
+    <t>dollar per victim</t>
+  </si>
+  <si>
+    <t>for total detainee population - need to divide it</t>
+  </si>
+  <si>
+    <t>n of all Detainees in 2018</t>
+  </si>
+  <si>
+    <t>n_jail_flow</t>
   </si>
 </sst>
 </file>
@@ -413,7 +441,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,6 +470,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -463,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -471,9 +506,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -778,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="158" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -824,16 +860,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -866,31 +902,31 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="O2" s="6" t="s">
+      <c r="H2" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="O2" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -908,13 +944,13 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>128</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I3" s="3">
         <v>973000</v>
@@ -935,18 +971,18 @@
         <v>21</v>
       </c>
       <c r="R3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -959,22 +995,22 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="H5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I5" s="3">
         <v>875000</v>
@@ -993,56 +1029,57 @@
         <v>21</v>
       </c>
       <c r="P5" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>104</v>
+      </c>
+      <c r="R5" t="s">
+        <v>25</v>
+      </c>
+      <c r="S5" t="s">
         <v>105</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="T5" t="s">
         <v>106</v>
-      </c>
-      <c r="R5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S5" t="s">
-        <v>107</v>
-      </c>
-      <c r="T5" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>128</v>
       </c>
       <c r="F7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G7" s="3">
         <v>2017</v>
@@ -1059,75 +1096,75 @@
       </c>
       <c r="M7" s="3"/>
       <c r="O7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>111</v>
+      </c>
+      <c r="R7" t="s">
+        <v>112</v>
+      </c>
+      <c r="S7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P7" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>113</v>
-      </c>
-      <c r="R7" t="s">
-        <v>114</v>
-      </c>
-      <c r="S7" t="s">
-        <v>115</v>
-      </c>
-      <c r="T7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="D8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="O8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>109</v>
+      <c r="I8" s="8"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="O8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
         <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G9">
         <v>2018</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3">
         <v>3677</v>
       </c>
       <c r="J9" s="2">
@@ -1144,29 +1181,29 @@
         <v>21</v>
       </c>
       <c r="Q9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
       <c r="F10" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10">
+        <v>35</v>
+      </c>
+      <c r="I10" s="3">
         <v>60.37</v>
       </c>
       <c r="J10" s="2"/>
@@ -1176,38 +1213,38 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="O10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" t="s">
         <v>44</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11">
+        <v>35</v>
+      </c>
+      <c r="I11" s="3">
         <v>0.61</v>
       </c>
       <c r="J11">
@@ -1219,44 +1256,47 @@
         <v>0.71</v>
       </c>
       <c r="O11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q11" t="s">
+        <v>47</v>
+      </c>
+      <c r="R11" t="s">
+        <v>48</v>
+      </c>
+      <c r="S11" t="s">
         <v>49</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>50</v>
-      </c>
-      <c r="S11" t="s">
-        <v>51</v>
-      </c>
-      <c r="T11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>55</v>
-      </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G12">
         <v>2011</v>
       </c>
-      <c r="I12">
+      <c r="H12" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I12" s="3">
         <v>11</v>
       </c>
       <c r="J12">
@@ -1268,35 +1308,35 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="O12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="R12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
-        <v>60</v>
-      </c>
       <c r="F13" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13">
+        <v>35</v>
+      </c>
+      <c r="I13" s="3">
         <v>4.9400000000000004</v>
       </c>
       <c r="J13" s="2"/>
@@ -1306,41 +1346,41 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="O13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P13" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>60</v>
+      </c>
+      <c r="R13" t="s">
         <v>61</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>62</v>
-      </c>
-      <c r="R13" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14">
+        <v>65</v>
+      </c>
+      <c r="I14" s="3">
         <v>99.44</v>
       </c>
       <c r="J14" s="2"/>
@@ -1348,32 +1388,32 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="O14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G15">
         <v>2022</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="3">
         <v>11</v>
       </c>
       <c r="J15" s="2"/>
@@ -1383,41 +1423,41 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="O15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
         <v>72</v>
       </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" t="s">
-        <v>74</v>
-      </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G16">
         <v>2021</v>
       </c>
       <c r="H16" t="s">
-        <v>75</v>
-      </c>
-      <c r="I16">
+        <v>73</v>
+      </c>
+      <c r="I16" s="3">
         <v>249634</v>
       </c>
       <c r="J16">
@@ -1429,38 +1469,38 @@
         <v>249634</v>
       </c>
       <c r="O16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" t="s">
         <v>76</v>
-      </c>
-      <c r="B17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" t="s">
-        <v>78</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>128</v>
       </c>
       <c r="F17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G17">
         <v>2017</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="3">
         <v>130</v>
       </c>
       <c r="J17" s="2"/>
@@ -1473,78 +1513,86 @@
         <v>21</v>
       </c>
       <c r="P17" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>78</v>
+      </c>
+      <c r="R17" t="s">
         <v>79</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>80</v>
-      </c>
-      <c r="R17" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" t="s">
         <v>82</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>83</v>
       </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" t="s">
-        <v>85</v>
-      </c>
       <c r="E18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G18">
         <v>2015</v>
       </c>
-      <c r="I18">
+      <c r="H18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I18" s="3">
         <v>50</v>
       </c>
       <c r="J18">
         <v>25</v>
       </c>
-      <c r="K18" s="2"/>
+      <c r="K18" s="2">
+        <v>50</v>
+      </c>
       <c r="L18" s="2"/>
       <c r="M18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" t="s">
         <v>83</v>
       </c>
-      <c r="C19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" t="s">
-        <v>85</v>
-      </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>128</v>
       </c>
       <c r="F19" t="s">
-        <v>120</v>
-      </c>
-      <c r="I19">
+        <v>118</v>
+      </c>
+      <c r="G19">
+        <v>2018</v>
+      </c>
+      <c r="I19" s="3">
         <v>300</v>
       </c>
       <c r="J19">
@@ -1556,38 +1604,44 @@
         <v>400</v>
       </c>
       <c r="O19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P19" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>89</v>
+      </c>
+      <c r="R19" t="s">
         <v>90</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>91</v>
-      </c>
-      <c r="R19" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F20" t="s">
-        <v>120</v>
-      </c>
-      <c r="I20">
+        <v>118</v>
+      </c>
+      <c r="G20">
+        <v>2018</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I20" s="3">
         <v>448677628</v>
       </c>
       <c r="J20">
@@ -1597,32 +1651,35 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="O20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="R20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" t="s">
         <v>97</v>
       </c>
-      <c r="B21" t="s">
+      <c r="E21" t="s">
         <v>98</v>
       </c>
-      <c r="C21" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" t="s">
-        <v>100</v>
-      </c>
       <c r="F21" t="s">
-        <v>120</v>
-      </c>
-      <c r="I21">
+        <v>118</v>
+      </c>
+      <c r="G21">
+        <v>2018</v>
+      </c>
+      <c r="I21" s="3">
         <v>33945</v>
       </c>
       <c r="J21" s="2"/>
@@ -1632,23 +1689,52 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
         <v>98</v>
       </c>
-      <c r="C22" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" t="s">
-        <v>100</v>
-      </c>
       <c r="F22" t="s">
-        <v>120</v>
-      </c>
-      <c r="I22" s="5">
+        <v>118</v>
+      </c>
+      <c r="G22">
+        <v>2018</v>
+      </c>
+      <c r="I22" s="3">
         <v>5171000</v>
       </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G23">
+        <v>2018</v>
+      </c>
+      <c r="I23" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
calculator and values updated
</commit_message>
<xml_diff>
--- a/Data/CCJ_quantified_values.xlsx
+++ b/Data/CCJ_quantified_values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/td/PycharmProjects/CCJ/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1080FC-A4AB-AF4F-8266-2CF9ACE7E23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56EA14A-4595-F040-822C-8FF4A1E80F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="133">
   <si>
     <t>row_var</t>
   </si>
@@ -425,13 +425,13 @@
     <t>dollar per victim</t>
   </si>
   <si>
-    <t>for total detainee population - need to divide it</t>
-  </si>
-  <si>
     <t>n of all Detainees in 2018</t>
   </si>
   <si>
     <t>n_jail_flow</t>
+  </si>
+  <si>
+    <t>needed to divide it with annual running detainee population</t>
   </si>
 </sst>
 </file>
@@ -816,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="158" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="158" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -984,8 +984,8 @@
       <c r="C4" t="s">
         <v>117</v>
       </c>
-      <c r="D4">
-        <v>4</v>
+      <c r="D4" t="s">
+        <v>120</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -1003,11 +1003,14 @@
       <c r="C5" t="s">
         <v>117</v>
       </c>
-      <c r="D5" t="s">
-        <v>120</v>
+      <c r="D5">
+        <v>4</v>
       </c>
       <c r="E5" t="s">
         <v>129</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
       </c>
       <c r="H5" t="s">
         <v>108</v>
@@ -1639,7 +1642,7 @@
         <v>2018</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I20" s="3">
         <v>448677628</v>
@@ -1712,13 +1715,13 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
         <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E23" t="s">
         <v>98</v>

</xml_diff>